<commit_message>
Descriptive statistik and visualization
</commit_message>
<xml_diff>
--- a/deskriptive_statistik.xlsx
+++ b/deskriptive_statistik.xlsx
@@ -7,7 +7,17 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Descriptive Stats" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Post Analysis" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Link Reactions" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Link Comments" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Link Shares" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Emoji Reactions" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Emoji Comments" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Emoji Shares" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Hashtag Reactions" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Hashtag Comments" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Hashtag Shares" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -757,4 +767,488 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Hashtag</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>82.62800565770863</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>59.81826568265683</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Hashtag</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>825.7284299858558</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>542.4261992619926</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Emoji %</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>62.1998883305416</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Hashtag %</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>60.52484645449469</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Link %</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>19.48632049134562</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Link</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>reactions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3225.99653259362</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3021.255014326648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Link</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>69.66504854368932</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>65.34097421203438</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Link</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>649.1331484049931</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>675.4441260744985</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Emoji</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>reactions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>2851.797636632201</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3389.262118491921</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Emoji</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>comments</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>55.56129985228952</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>76.88150807899461</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Emoji</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>shares</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>583.6189069423929</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>697.1903052064632</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Contains Hashtag</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>reactions</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>3928.517680339462</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2701.884686346863</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>